<commit_message>
methodlength bug fixed, first gloassary
</commit_message>
<xml_diff>
--- a/text/images/performance.xlsx
+++ b/text/images/performance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CciAst</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Assemblies</t>
+  </si>
+  <si>
+    <t>Mescor</t>
   </si>
 </sst>
 </file>
@@ -183,53 +186,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Zeiten!$A$2:$A$7</c:f>
+              <c:f>Zeiten!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Mescor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Usus.net (mit PDBs)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Usus.net (ohne PDBs)</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>CciAst</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>CciMetadata</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>GraphSharp</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>QuickGraph</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Usus.net (mit PDBs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Usus.net (ohne PDBs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Zeiten!$D$2:$D$7</c:f>
+              <c:f>Zeiten!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>176.49600000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.708670699999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.4356434</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>124.8193996</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>38.4668463</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>8.2278227000000008</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>4.6634662999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.708670699999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16.4356434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -252,53 +261,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Zeiten!$A$2:$A$7</c:f>
+              <c:f>Zeiten!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Mescor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Usus.net (mit PDBs)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Usus.net (ohne PDBs)</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>CciAst</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>CciMetadata</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>GraphSharp</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>QuickGraph</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Usus.net (mit PDBs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Usus.net (ohne PDBs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Zeiten!$E$2:$E$7</c:f>
+              <c:f>Zeiten!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>158.5880626</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.8075806</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.5455544</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>68.749874300000002</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>28.202819999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>7.6147613999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>4.6054605000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.8075806</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15.5455544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -313,11 +328,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195768320"/>
-        <c:axId val="47997312"/>
+        <c:axId val="177177728"/>
+        <c:axId val="177179264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195768320"/>
+        <c:axId val="177177728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,7 +341,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47997312"/>
+        <c:crossAx val="177179264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -334,7 +349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47997312"/>
+        <c:axId val="177179264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,7 +379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195768320"/>
+        <c:crossAx val="177177728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -453,53 +468,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Zeiten!$A$2:$A$7</c:f>
+              <c:f>Zeiten!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Mescor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Usus.net (mit PDBs)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Usus.net (ohne PDBs)</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>CciAst</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>CciMetadata</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>GraphSharp</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>QuickGraph</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Usus.net (mit PDBs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Usus.net (ohne PDBs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Zeiten!$B$2:$B$7</c:f>
+              <c:f>Zeiten!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -514,8 +535,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="251434496"/>
-        <c:axId val="251436416"/>
+        <c:axId val="115946624"/>
+        <c:axId val="115948160"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -538,53 +559,59 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Zeiten!$A$2:$A$7</c:f>
+              <c:f>Zeiten!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Mescor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Usus.net (mit PDBs)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Usus.net (ohne PDBs)</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>CciAst</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>CciMetadata</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>GraphSharp</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>QuickGraph</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Usus.net (mit PDBs)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Usus.net (ohne PDBs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Zeiten!$C$2:$C$7</c:f>
+              <c:f>Zeiten!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>79098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5613</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5613</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>118826</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>63082</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>7731</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>18909</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5613</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5613</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,11 +626,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="206009088"/>
-        <c:axId val="196270336"/>
+        <c:axId val="115956352"/>
+        <c:axId val="115954432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251434496"/>
+        <c:axId val="115946624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +639,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251436416"/>
+        <c:crossAx val="115948160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +647,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251436416"/>
+        <c:axId val="115948160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,12 +677,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251434496"/>
+        <c:crossAx val="115946624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196270336"/>
+        <c:axId val="115954432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -684,12 +711,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206009088"/>
+        <c:crossAx val="115956352"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="206009088"/>
+        <c:axId val="115956352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +725,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196270336"/>
+        <c:crossAx val="115954432"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -707,7 +735,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76336597834693298"/>
+          <c:y val="0.91202591247951315"/>
+          <c:w val="0.23267871478214969"/>
+          <c:h val="6.6056285605641793E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -788,8 +825,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Projekt"/>
     <tableColumn id="5" name="Assemblies" dataDxfId="3"/>
@@ -1088,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,104 +1159,121 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1">
-        <v>118826</v>
+        <v>79098</v>
       </c>
       <c r="D2" s="1">
-        <v>124.8193996</v>
+        <v>176.49600000000001</v>
       </c>
       <c r="E2" s="1">
-        <v>68.749874300000002</v>
+        <v>158.5880626</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
-        <v>63082</v>
+        <v>5613</v>
       </c>
       <c r="D3" s="1">
-        <v>38.4668463</v>
+        <v>16.708670699999999</v>
       </c>
       <c r="E3" s="1">
-        <v>28.202819999999999</v>
+        <v>15.8075806</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>7731</v>
+        <v>5613</v>
       </c>
       <c r="D4" s="1">
-        <v>8.2278227000000008</v>
+        <v>16.4356434</v>
       </c>
       <c r="E4" s="1">
-        <v>7.6147613999999999</v>
+        <v>15.5455544</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
-        <v>18909</v>
+        <v>118826</v>
       </c>
       <c r="D5" s="1">
-        <v>4.6634662999999996</v>
+        <v>124.8193996</v>
       </c>
       <c r="E5" s="1">
-        <v>4.6054605000000004</v>
+        <v>68.749874300000002</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>5613</v>
+        <v>63082</v>
       </c>
       <c r="D6" s="1">
-        <v>16.708670699999999</v>
+        <v>38.4668463</v>
       </c>
       <c r="E6" s="1">
-        <v>15.8075806</v>
+        <v>28.202819999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>5613</v>
+        <v>7731</v>
       </c>
       <c r="D7" s="1">
-        <v>16.4356434</v>
+        <v>8.2278227000000008</v>
       </c>
       <c r="E7" s="1">
-        <v>15.5455544</v>
+        <v>7.6147613999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>18909</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.6634662999999996</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4.6054605000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>